<commit_message>
Updated structures test list
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\rom-folderer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F624D9-7A1B-459D-9ECD-0AC88F704A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BADF67-6730-4316-9B8C-09A986AF20C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{09D53552-1463-4F16-9BD4-A353FB5A1398}"/>
+    <workbookView xWindow="20280" yWindow="14910" windowWidth="23760" windowHeight="15510" activeTab="1" xr2:uid="{09D53552-1463-4F16-9BD4-A353FB5A1398}"/>
   </bookViews>
   <sheets>
     <sheet name="Systems" sheetId="1" r:id="rId1"/>
@@ -469,7 +469,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F045E33-1671-4698-A15E-5993233E5D1E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -530,7 +532,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +558,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -567,7 +569,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -578,7 +580,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -589,7 +591,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Added Atari VCS keyword
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\rom-folderer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB85C6AC-5422-42FA-828C-3C937F5C34A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC6257B-9C7E-4552-9746-5C4C6436FD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28170" yWindow="8265" windowWidth="23760" windowHeight="15510" activeTab="1" xr2:uid="{09D53552-1463-4F16-9BD4-A353FB5A1398}"/>
+    <workbookView xWindow="19320" yWindow="4770" windowWidth="24750" windowHeight="17355" xr2:uid="{09D53552-1463-4F16-9BD4-A353FB5A1398}"/>
   </bookViews>
   <sheets>
     <sheet name="Systems" sheetId="1" r:id="rId1"/>
@@ -849,15 +849,9 @@
     <t>a800,a800</t>
   </si>
   <si>
-    <t>7800,a7800</t>
-  </si>
-  <si>
     <t>jaguarcd,jagual-cd</t>
   </si>
   <si>
-    <t>5200,a5200</t>
-  </si>
-  <si>
     <t>macos</t>
   </si>
   <si>
@@ -930,10 +924,16 @@
     <t>mame</t>
   </si>
   <si>
-    <t>2600,vcs</t>
-  </si>
-  <si>
     <t>Playstatio 1</t>
+  </si>
+  <si>
+    <t>2600,vcs,atari2600</t>
+  </si>
+  <si>
+    <t>5200,a5200,atari5200</t>
+  </si>
+  <si>
+    <t>7800,a7800,atari7800</t>
   </si>
 </sst>
 </file>
@@ -1333,8 +1333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F045E33-1671-4698-A15E-5993233E5D1E}">
   <dimension ref="A1:B164"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,7 +1356,7 @@
         <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1406,7 +1406,7 @@
         <v>160</v>
       </c>
       <c r="B9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1424,7 +1424,7 @@
         <v>158</v>
       </c>
       <c r="B12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1448,7 +1448,7 @@
         <v>156</v>
       </c>
       <c r="B15" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1456,7 +1456,7 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1464,7 +1464,7 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1472,7 +1472,7 @@
         <v>154</v>
       </c>
       <c r="B18" t="s">
-        <v>272</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1480,7 +1480,7 @@
         <v>153</v>
       </c>
       <c r="B19" t="s">
-        <v>270</v>
+        <v>298</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1504,7 +1504,7 @@
         <v>150</v>
       </c>
       <c r="B22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1637,10 +1637,10 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B42" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2100,7 +2100,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B113" t="s">
         <v>253</v>
@@ -2512,8 +2512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD1930EB-6B5A-4138-8372-6C9155206B66}">
   <dimension ref="A1:C185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
-      <selection activeCell="B183" sqref="B183"/>
+    <sheetView topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="B168" sqref="B168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -2558,7 +2558,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -2569,7 +2569,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -2580,7 +2580,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -2591,7 +2591,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -2602,7 +2602,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -2613,7 +2613,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -2635,7 +2635,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -2646,7 +2646,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
@@ -2657,7 +2657,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
@@ -2668,7 +2668,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B14" t="s">
         <v>19</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
@@ -2690,7 +2690,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
@@ -2701,7 +2701,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
@@ -2712,7 +2712,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B18" t="s">
         <v>23</v>
@@ -2723,7 +2723,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B19" t="s">
         <v>24</v>
@@ -2734,7 +2734,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
@@ -2745,7 +2745,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
@@ -2756,7 +2756,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B22" t="s">
         <v>27</v>
@@ -2767,7 +2767,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B23" t="s">
         <v>28</v>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B24" t="s">
         <v>29</v>
@@ -2789,7 +2789,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B25" t="s">
         <v>30</v>
@@ -2800,7 +2800,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B26" t="s">
         <v>31</v>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B27" t="s">
         <v>32</v>
@@ -2822,7 +2822,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B28" t="s">
         <v>33</v>
@@ -2833,7 +2833,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B29" t="s">
         <v>34</v>
@@ -2844,7 +2844,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B30" t="s">
         <v>230</v>
@@ -2855,7 +2855,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B31" t="s">
         <v>35</v>
@@ -2866,7 +2866,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B32" t="s">
         <v>36</v>
@@ -2877,7 +2877,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B33" t="s">
         <v>37</v>
@@ -2888,7 +2888,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B34" t="s">
         <v>38</v>
@@ -2899,7 +2899,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B35" t="s">
         <v>39</v>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B36" t="s">
         <v>40</v>
@@ -2921,7 +2921,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B37" t="s">
         <v>41</v>
@@ -2932,7 +2932,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B38" t="s">
         <v>42</v>
@@ -2943,7 +2943,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B39" t="s">
         <v>43</v>
@@ -2954,7 +2954,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B40" t="s">
         <v>44</v>
@@ -2965,7 +2965,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B41" t="s">
         <v>45</v>
@@ -2976,7 +2976,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B42" t="s">
         <v>46</v>
@@ -2987,7 +2987,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B43" t="s">
         <v>47</v>
@@ -2998,7 +2998,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B44" t="s">
         <v>48</v>
@@ -3009,7 +3009,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B45" t="s">
         <v>49</v>
@@ -3020,7 +3020,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B46" t="s">
         <v>50</v>
@@ -3031,7 +3031,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B47" t="s">
         <v>51</v>
@@ -3042,7 +3042,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B48" t="s">
         <v>52</v>
@@ -3053,7 +3053,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B49" t="s">
         <v>53</v>
@@ -3064,7 +3064,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B50" t="s">
         <v>54</v>
@@ -3075,7 +3075,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B51" t="s">
         <v>55</v>
@@ -3086,7 +3086,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B52" t="s">
         <v>56</v>
@@ -3097,7 +3097,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B53" t="s">
         <v>57</v>
@@ -3108,7 +3108,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B54" t="s">
         <v>58</v>
@@ -3119,7 +3119,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B55" t="s">
         <v>59</v>
@@ -3130,7 +3130,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B56" t="s">
         <v>60</v>
@@ -3141,7 +3141,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B57" t="s">
         <v>61</v>
@@ -3152,7 +3152,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B58" t="s">
         <v>62</v>
@@ -3163,7 +3163,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B59" t="s">
         <v>63</v>
@@ -3174,7 +3174,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B60" t="s">
         <v>64</v>
@@ -3185,7 +3185,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B61" t="s">
         <v>65</v>
@@ -3196,7 +3196,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B62" t="s">
         <v>66</v>
@@ -3207,7 +3207,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B63" t="s">
         <v>67</v>
@@ -3218,7 +3218,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B64" t="s">
         <v>68</v>
@@ -3229,7 +3229,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B65" t="s">
         <v>69</v>
@@ -3240,7 +3240,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B66" t="s">
         <v>70</v>
@@ -3251,7 +3251,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B67" t="s">
         <v>71</v>
@@ -3262,7 +3262,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B68" t="s">
         <v>72</v>
@@ -3273,7 +3273,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B69" t="s">
         <v>73</v>
@@ -3284,7 +3284,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B70" t="s">
         <v>74</v>
@@ -3295,7 +3295,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B71" t="s">
         <v>75</v>
@@ -3306,7 +3306,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B72" t="s">
         <v>76</v>
@@ -3317,7 +3317,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B73" t="s">
         <v>77</v>
@@ -3328,7 +3328,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B74" t="s">
         <v>78</v>
@@ -3339,7 +3339,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B75" t="s">
         <v>79</v>
@@ -3350,7 +3350,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B76" t="s">
         <v>80</v>
@@ -3361,7 +3361,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B77" t="s">
         <v>81</v>
@@ -3372,7 +3372,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B78" t="s">
         <v>82</v>
@@ -3383,7 +3383,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B79" t="s">
         <v>83</v>
@@ -3394,7 +3394,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B80" t="s">
         <v>84</v>
@@ -3405,7 +3405,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B81" t="s">
         <v>85</v>
@@ -3416,7 +3416,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B82" t="s">
         <v>86</v>
@@ -3427,7 +3427,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B83" t="s">
         <v>87</v>
@@ -3438,7 +3438,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B84" t="s">
         <v>88</v>
@@ -3449,7 +3449,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B85" t="s">
         <v>89</v>
@@ -3460,7 +3460,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B86" t="s">
         <v>90</v>
@@ -3471,7 +3471,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B87" t="s">
         <v>91</v>
@@ -3482,7 +3482,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B88" t="s">
         <v>92</v>
@@ -3493,7 +3493,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B89" t="s">
         <v>93</v>
@@ -3504,7 +3504,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B90" t="s">
         <v>94</v>
@@ -3515,7 +3515,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B91" t="s">
         <v>95</v>
@@ -3526,7 +3526,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B92" t="s">
         <v>96</v>
@@ -3537,7 +3537,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B93" t="s">
         <v>97</v>
@@ -3548,7 +3548,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B94" t="s">
         <v>98</v>
@@ -3559,7 +3559,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B95" t="s">
         <v>99</v>
@@ -3570,7 +3570,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B96" t="s">
         <v>100</v>
@@ -3581,7 +3581,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B97" t="s">
         <v>101</v>
@@ -3592,7 +3592,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B98" t="s">
         <v>102</v>
@@ -3603,7 +3603,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B99" t="s">
         <v>103</v>
@@ -3614,7 +3614,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B100" t="s">
         <v>104</v>
@@ -3625,7 +3625,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B101" t="s">
         <v>105</v>
@@ -3636,7 +3636,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B102" t="s">
         <v>106</v>
@@ -3647,7 +3647,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B103" t="s">
         <v>107</v>
@@ -3658,7 +3658,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B104" t="s">
         <v>108</v>
@@ -3669,7 +3669,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B105" t="s">
         <v>109</v>
@@ -3680,7 +3680,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B106" t="s">
         <v>110</v>
@@ -3691,7 +3691,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B107" t="s">
         <v>111</v>
@@ -3702,7 +3702,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B108" t="s">
         <v>112</v>
@@ -3713,7 +3713,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B109" t="s">
         <v>113</v>
@@ -3724,7 +3724,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B110" t="s">
         <v>114</v>
@@ -3735,7 +3735,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B111" t="s">
         <v>115</v>
@@ -3746,7 +3746,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B112" t="s">
         <v>116</v>
@@ -3757,7 +3757,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B113" t="s">
         <v>117</v>
@@ -3768,7 +3768,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B114" t="s">
         <v>118</v>
@@ -3779,7 +3779,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B115" t="s">
         <v>119</v>
@@ -3790,7 +3790,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B116" t="s">
         <v>120</v>
@@ -3801,7 +3801,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B117" t="s">
         <v>121</v>
@@ -3812,7 +3812,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B118" t="s">
         <v>122</v>
@@ -3823,7 +3823,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B119" t="s">
         <v>123</v>
@@ -3834,7 +3834,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B120" t="s">
         <v>124</v>
@@ -3845,7 +3845,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B121" t="s">
         <v>125</v>
@@ -3856,7 +3856,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B122" t="s">
         <v>126</v>
@@ -3867,7 +3867,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B123" t="s">
         <v>127</v>
@@ -3878,7 +3878,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B124" t="s">
         <v>128</v>
@@ -3889,7 +3889,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B125" t="s">
         <v>129</v>
@@ -3900,7 +3900,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B126" t="s">
         <v>130</v>
@@ -3911,7 +3911,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B127" t="s">
         <v>131</v>
@@ -3922,7 +3922,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B128" t="s">
         <v>132</v>
@@ -3933,7 +3933,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B129" t="s">
         <v>133</v>
@@ -3944,7 +3944,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B130" t="s">
         <v>134</v>
@@ -3955,7 +3955,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B131" t="s">
         <v>135</v>
@@ -3966,7 +3966,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B132" t="s">
         <v>136</v>
@@ -3977,7 +3977,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B133" t="s">
         <v>137</v>
@@ -3988,7 +3988,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B134" t="s">
         <v>138</v>
@@ -3999,7 +3999,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B135" t="s">
         <v>139</v>
@@ -4010,7 +4010,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B136" t="s">
         <v>140</v>
@@ -4021,7 +4021,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B137" t="s">
         <v>141</v>
@@ -4032,7 +4032,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B138" t="s">
         <v>142</v>
@@ -4043,7 +4043,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B139" t="s">
         <v>143</v>
@@ -4054,7 +4054,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B140" t="s">
         <v>144</v>
@@ -4065,7 +4065,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B141" t="s">
         <v>145</v>
@@ -4076,7 +4076,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B142" t="s">
         <v>146</v>
@@ -4087,7 +4087,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B143" t="s">
         <v>147</v>
@@ -4098,7 +4098,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B144" t="s">
         <v>148</v>
@@ -4109,7 +4109,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B145" t="s">
         <v>149</v>
@@ -4120,7 +4120,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B146" t="s">
         <v>150</v>
@@ -4131,7 +4131,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B147" t="s">
         <v>151</v>
@@ -4142,7 +4142,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B148" t="s">
         <v>152</v>
@@ -4153,7 +4153,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B149" t="s">
         <v>153</v>
@@ -4164,7 +4164,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B150" t="s">
         <v>154</v>
@@ -4175,7 +4175,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B151" t="s">
         <v>155</v>
@@ -4186,7 +4186,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B152" t="s">
         <v>156</v>
@@ -4197,7 +4197,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B153" t="s">
         <v>157</v>
@@ -4208,7 +4208,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B154" t="s">
         <v>158</v>
@@ -4219,7 +4219,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B155" t="s">
         <v>159</v>
@@ -4230,7 +4230,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B156" t="s">
         <v>160</v>
@@ -4241,7 +4241,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B157" t="s">
         <v>161</v>
@@ -4252,7 +4252,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B158" t="s">
         <v>162</v>
@@ -4263,7 +4263,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B159" t="s">
         <v>163</v>
@@ -4274,7 +4274,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B160" t="s">
         <v>164</v>
@@ -4285,7 +4285,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B161" t="s">
         <v>165</v>
@@ -4296,7 +4296,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B162" t="s">
         <v>166</v>
@@ -4307,7 +4307,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B163" t="s">
         <v>167</v>
@@ -4318,7 +4318,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B164" t="s">
         <v>168</v>
@@ -4346,7 +4346,7 @@
         <v>11</v>
       </c>
       <c r="C166" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -4368,7 +4368,7 @@
         <v>20</v>
       </c>
       <c r="C168" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -4387,10 +4387,10 @@
         <v>7</v>
       </c>
       <c r="B170" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C170" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -4401,7 +4401,7 @@
         <v>12</v>
       </c>
       <c r="C171" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -4412,7 +4412,7 @@
         <v>14</v>
       </c>
       <c r="C172" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -4423,7 +4423,7 @@
         <v>13</v>
       </c>
       <c r="C173" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -4434,7 +4434,7 @@
         <v>15</v>
       </c>
       <c r="C174" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -4442,10 +4442,10 @@
         <v>7</v>
       </c>
       <c r="B175" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C175" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -4456,7 +4456,7 @@
         <v>26</v>
       </c>
       <c r="C176" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -4467,7 +4467,7 @@
         <v>91</v>
       </c>
       <c r="C177" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -4478,7 +4478,7 @@
         <v>16</v>
       </c>
       <c r="C178" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -4489,7 +4489,7 @@
         <v>17</v>
       </c>
       <c r="C179" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -4500,7 +4500,7 @@
         <v>21</v>
       </c>
       <c r="C180" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -4511,7 +4511,7 @@
         <v>27</v>
       </c>
       <c r="C181" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -4522,7 +4522,7 @@
         <v>19</v>
       </c>
       <c r="C182" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -4533,7 +4533,7 @@
         <v>22</v>
       </c>
       <c r="C183" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -4544,7 +4544,7 @@
         <v>23</v>
       </c>
       <c r="C184" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -4552,10 +4552,10 @@
         <v>7</v>
       </c>
       <c r="B185" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C185" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>